<commit_message>
Agregando modulo de correos
</commit_message>
<xml_diff>
--- a/factura.xlsx
+++ b/factura.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,24 +468,288 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>2024-01</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Vj9W-c4Pm-ja0X-fC1C</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>20157</v>
+      </c>
+      <c r="D2" t="n">
+        <v>4998</v>
+      </c>
+      <c r="E2" t="n">
+        <v>4526690</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2024-02</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Vj9W-c4Pm-ja0X-fC1C</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>18768</v>
+      </c>
+      <c r="D3" t="n">
+        <v>4737</v>
+      </c>
+      <c r="E3" t="n">
+        <v>4253600</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2024-03</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Vj9W-c4Pm-ja0X-fC1C</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>20518</v>
+      </c>
+      <c r="D4" t="n">
+        <v>5045</v>
+      </c>
+      <c r="E4" t="n">
+        <v>4588060</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2024-04</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Vj9W-c4Pm-ja0X-fC1C</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>19861</v>
+      </c>
+      <c r="D5" t="n">
+        <v>4966</v>
+      </c>
+      <c r="E5" t="n">
+        <v>4472200</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2024-05</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Vj9W-c4Pm-ja0X-fC1C</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>20352</v>
+      </c>
+      <c r="D6" t="n">
+        <v>5093</v>
+      </c>
+      <c r="E6" t="n">
+        <v>4559840</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2024-06</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Vj9W-c4Pm-ja0X-fC1C</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>19705</v>
+      </c>
+      <c r="D7" t="n">
+        <v>4913</v>
+      </c>
+      <c r="E7" t="n">
+        <v>4441000</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2024-07</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Vj9W-c4Pm-ja0X-fC1C</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>20387</v>
+      </c>
+      <c r="D8" t="n">
+        <v>5029</v>
+      </c>
+      <c r="E8" t="n">
+        <v>4565790</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2024-08</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Vj9W-c4Pm-ja0X-fC1C</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>20358</v>
+      </c>
+      <c r="D9" t="n">
+        <v>5030</v>
+      </c>
+      <c r="E9" t="n">
+        <v>4560860</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2024-09</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Vj9W-c4Pm-ja0X-fC1C</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>19907</v>
+      </c>
+      <c r="D10" t="n">
+        <v>4838</v>
+      </c>
+      <c r="E10" t="n">
+        <v>4481400</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
           <t>2024-10</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Vj9W-c4Pm-ja0X-fC1C</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Vj9W-c4Pm-ja0X-fC1C</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
         <v>20440</v>
       </c>
-      <c r="D2" t="n">
+      <c r="D11" t="n">
         <v>5137</v>
       </c>
-      <c r="E2" t="n">
+      <c r="E11" t="n">
         <v>4574800</v>
       </c>
-      <c r="F2" t="n">
+      <c r="F11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2024-11</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Vj9W-c4Pm-ja0X-fC1C</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>19651</v>
+      </c>
+      <c r="D12" t="n">
+        <v>4793</v>
+      </c>
+      <c r="E12" t="n">
+        <v>4430200</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2024-12</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Vj9W-c4Pm-ja0X-fC1C</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>20281</v>
+      </c>
+      <c r="D13" t="n">
+        <v>4991</v>
+      </c>
+      <c r="E13" t="n">
+        <v>4547770</v>
+      </c>
+      <c r="F13" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Se actualiza el modulo load_4 y se agrega el README
</commit_message>
<xml_diff>
--- a/factura.xlsx
+++ b/factura.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,7 +468,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2024-01</t>
+          <t>2024-10</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -477,279 +477,15 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>20157</v>
+        <v>20440</v>
       </c>
       <c r="D2" t="n">
-        <v>4998</v>
+        <v>5137</v>
       </c>
       <c r="E2" t="n">
-        <v>4526690</v>
+        <v>4574800</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2024-02</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Vj9W-c4Pm-ja0X-fC1C</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>18768</v>
-      </c>
-      <c r="D3" t="n">
-        <v>4737</v>
-      </c>
-      <c r="E3" t="n">
-        <v>4253600</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>2024-03</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Vj9W-c4Pm-ja0X-fC1C</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>20518</v>
-      </c>
-      <c r="D4" t="n">
-        <v>5045</v>
-      </c>
-      <c r="E4" t="n">
-        <v>4588060</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>2024-04</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Vj9W-c4Pm-ja0X-fC1C</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>19861</v>
-      </c>
-      <c r="D5" t="n">
-        <v>4966</v>
-      </c>
-      <c r="E5" t="n">
-        <v>4472200</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>2024-05</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Vj9W-c4Pm-ja0X-fC1C</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>20352</v>
-      </c>
-      <c r="D6" t="n">
-        <v>5093</v>
-      </c>
-      <c r="E6" t="n">
-        <v>4559840</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>2024-06</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Vj9W-c4Pm-ja0X-fC1C</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>19705</v>
-      </c>
-      <c r="D7" t="n">
-        <v>4913</v>
-      </c>
-      <c r="E7" t="n">
-        <v>4441000</v>
-      </c>
-      <c r="F7" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>2024-07</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Vj9W-c4Pm-ja0X-fC1C</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>20387</v>
-      </c>
-      <c r="D8" t="n">
-        <v>5029</v>
-      </c>
-      <c r="E8" t="n">
-        <v>4565790</v>
-      </c>
-      <c r="F8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>2024-08</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Vj9W-c4Pm-ja0X-fC1C</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
-        <v>20358</v>
-      </c>
-      <c r="D9" t="n">
-        <v>5030</v>
-      </c>
-      <c r="E9" t="n">
-        <v>4560860</v>
-      </c>
-      <c r="F9" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>2024-09</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Vj9W-c4Pm-ja0X-fC1C</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>19907</v>
-      </c>
-      <c r="D10" t="n">
-        <v>4838</v>
-      </c>
-      <c r="E10" t="n">
-        <v>4481400</v>
-      </c>
-      <c r="F10" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>2024-10</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Vj9W-c4Pm-ja0X-fC1C</t>
-        </is>
-      </c>
-      <c r="C11" t="n">
-        <v>20440</v>
-      </c>
-      <c r="D11" t="n">
-        <v>5137</v>
-      </c>
-      <c r="E11" t="n">
-        <v>4574800</v>
-      </c>
-      <c r="F11" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>2024-11</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Vj9W-c4Pm-ja0X-fC1C</t>
-        </is>
-      </c>
-      <c r="C12" t="n">
-        <v>19651</v>
-      </c>
-      <c r="D12" t="n">
-        <v>4793</v>
-      </c>
-      <c r="E12" t="n">
-        <v>4430200</v>
-      </c>
-      <c r="F12" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>2024-12</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Vj9W-c4Pm-ja0X-fC1C</t>
-        </is>
-      </c>
-      <c r="C13" t="n">
-        <v>20281</v>
-      </c>
-      <c r="D13" t="n">
-        <v>4991</v>
-      </c>
-      <c r="E13" t="n">
-        <v>4547770</v>
-      </c>
-      <c r="F13" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>